<commit_message>
final commit for June branch
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Canine_StudyDetailPage_StudyFiles_Tab.xlsx
+++ b/InputFiles/TC01_Canine_StudyDetailPage_StudyFiles_Tab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\June\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2797A0-96C1-4B70-82CA-7A294E66DBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94E04AA-EBE6-4AE6-BC38-7297D52FA8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -58,22 +58,20 @@
     <t>TC01_Canine_StudyDetailPage_StudyFiles_Tab_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(s:study)
-MATCH (s)&lt;--(c:case)&lt;--(diag:diagnosis)
-MATCH (samp:sample)--&gt;(c)
-MATCH (c)&lt;--(demo:demographic)
-MATCH (f:file)--&gt;(parent)
-WHERE s.clinical_study_designation IN['NCATS-COP01'] 
+    <t xml:space="preserve">  MATCH (f:file)--&gt;(s:study)
+MATCH (s)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis)
+WHERE s.clinical_study_designation  IN ['NCATS-COP01'] 
+WITH DISTINCT f,  s, c, demo, diag
 WITH
-        DISTINCT f, c, demo, diag, s,
+        f, c, demo, diag, s,
         ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
         toInteger(floor(log(f.file_size)/log(1024))) as i,
         2 as precision
-WITH
+WITH    
         f, c, demo, diag, s,
         f.file_size /(1024^i) AS value, 10^precision AS factor,
         units[i] as unit
-        WITH
+        WITH    
         f,  c, demo, diag, s, unit,
         round(factor * value)/factor AS size
 RETURN DISTINCT
@@ -82,19 +80,19 @@
   coalesce("study", '') AS `Association`,
   coalesce(f.file_description, '') AS `Description`,
   coalesce(f.file_format, '') AS  Format,
-  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-  order by 'File Name' asc
-  limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+  CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size
+Order By `File Name` LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)
+WHERE s.clinical_study_designation IN['NCATS-COP01']
+MATCH (p:program)&lt;--(s)&lt;--(c:case)
+OPTIONAL MATCH (demo:demographic)--&gt;(c)
 OPTIONAL MATCH (samp:sample)--&gt;(c)
 OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
-OPTIONAL MATCH (cf:file)-[*]-&gt;(samp)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-WITH DISTINCT cf, sf, samp AS samp, c, demo, diag, s, p
-WHERE s.clinical_study_designation IN['NCATS-COP01']
-RETURN  
+OPTIONAL MATCH (cf:file)-[*]-&gt;(c)
+OPTIONAL  MATCH (sf:file)--&gt;(s)
+RETURN
     count(distinct p) AS Programs,
     count(distinct s) AS Studies,
     count(distinct c) AS Cases,
@@ -481,19 +479,19 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.42578125" customWidth="1"/>
-    <col min="3" max="3" width="86.140625" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.453125" customWidth="1"/>
+    <col min="3" max="3" width="86.1796875" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="40.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -510,7 +508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -540,7 +538,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>